<commit_message>
Actualización archivo pruebas backend
</commit_message>
<xml_diff>
--- a/Documentación/Pruebas_backend.xlsx
+++ b/Documentación/Pruebas_backend.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SC_701_ProyectoFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SC_701_ProyectoFinal\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23F64304-C218-47EB-BB1C-595B8A55A55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7376CD30-6FE9-48FC-B6E9-8D722FC8F63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F94651A-E338-42BA-B105-25686463F0FA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>TABLAS</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>Funciona</t>
-  </si>
-  <si>
-    <t>Revision</t>
   </si>
   <si>
     <t>Notas</t>
@@ -123,18 +120,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -260,14 +251,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -282,11 +269,177 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -318,167 +471,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -493,15 +485,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDD8CADC-86E3-458F-BF02-670112CC1211}" name="Tabla1" displayName="Tabla1" ref="B5:G14" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDD8CADC-86E3-458F-BF02-670112CC1211}" name="Tabla1" displayName="Tabla1" ref="B5:G14" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B5:G14" xr:uid="{BDD8CADC-86E3-458F-BF02-670112CC1211}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7998F1A2-B2CC-4B38-BDB8-CEB5908FD727}" name="TABLAS" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C9C65EB2-DA6D-4399-9E9A-991279B703CD}" name="GET" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DDEF08C7-77CB-42CA-8372-E85EB38A8A27}" name="GET_ID" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{92181635-79A4-4334-A4C8-4DAA0C8A17E9}" name="POST" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D83A2262-C111-46E1-B750-7FACBF95A02F}" name="PUT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B267EF69-125B-451D-8612-396936283664}" name="DELETE" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7998F1A2-B2CC-4B38-BDB8-CEB5908FD727}" name="TABLAS" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C9C65EB2-DA6D-4399-9E9A-991279B703CD}" name="GET" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DDEF08C7-77CB-42CA-8372-E85EB38A8A27}" name="GET_ID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{92181635-79A4-4334-A4C8-4DAA0C8A17E9}" name="POST" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D83A2262-C111-46E1-B750-7FACBF95A02F}" name="PUT" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B267EF69-125B-451D-8612-396936283664}" name="DELETE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -804,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128E47C6-9ED4-4784-A489-A743E08E7D00}">
-  <dimension ref="B5:Q14"/>
+  <dimension ref="A5:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,248 +808,249 @@
     <col min="10" max="10" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="C7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="C9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="C10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="C12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>